<commit_message>
Se puede enviar mensajes y guardar en la base de datos, en mensajes/add
</commit_message>
<xml_diff>
--- a/chats/51958232911@c.us.xlsx
+++ b/chats/51958232911@c.us.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Fecha</t>
   </si>
@@ -44,6 +44,65 @@
   </si>
   <si>
     <t>Mensaje respondido desde la API 2</t>
+  </si>
+  <si>
+    <t>14-06-2021 03:45</t>
+  </si>
+  <si>
+    <t>p de mensaje 2</t>
+  </si>
+  <si>
+    <t>14-06-2021 03:52</t>
+  </si>
+  <si>
+    <t>14-06-2021 03:58</t>
+  </si>
+  <si>
+    <t>Paso 02</t>
+  </si>
+  <si>
+    <t>14-06-2021 04:01</t>
+  </si>
+  <si>
+    <t>14-06-2021 04:02</t>
+  </si>
+  <si>
+    <t>14-06-2021 04:03</t>
+  </si>
+  <si>
+    <t>hola prueba desde poooosmmaaaan</t>
+  </si>
+  <si>
+    <t>14-06-2021 04:04</t>
+  </si>
+  <si>
+    <t>Prueba - Mandando mensaje y agregando a la base de datos</t>
+  </si>
+  <si>
+    <t>14-06-2021 04:06</t>
+  </si>
+  <si>
+    <t>14-06-2021 04:07</t>
+  </si>
+  <si>
+    <t>Prueba - Mandando mensaje y agregando a la base de datos 2</t>
+  </si>
+  <si>
+    <t>Prueba - Mandando mensaje y agregando a la base de datos 3</t>
+  </si>
+  <si>
+    <t>14-06-2021 04:08</t>
+  </si>
+  <si>
+    <t>Hola Bienvenido\n\nEste es un mensaje de Prueba. Deberás enviarnos el *numero* de lo que estas buscando.\n*1*. Opción 1\n*2*. Opción 2\n*3*. Opción 3\n\nDeberás enviar el *número* de la opción solicitado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hola Bienvenido
+Este es un mensaje de Prueba. Deberás enviarnos el *numero* de lo que estas buscando
+*1*. Opción 1
+*2*. Opción 2
+*3*. Opción 3
+Deberás enviar el *número* de la opción solicitado.</t>
   </si>
 </sst>
 </file>
@@ -420,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B21"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -495,6 +554,102 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>